<commit_message>
Almost done with draft one?
</commit_message>
<xml_diff>
--- a/DataFiles/Data_study/Data_analysis.xlsx
+++ b/DataFiles/Data_study/Data_analysis.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="People" sheetId="2" r:id="rId2"/>
+    <sheet name="LOOCV DATA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Train #</t>
   </si>
@@ -67,6 +68,9 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>20_4mo</t>
   </si>
 </sst>
 </file>
@@ -289,11 +293,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359356112"/>
-        <c:axId val="359961168"/>
+        <c:axId val="423791936"/>
+        <c:axId val="423768416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="359356112"/>
+        <c:axId val="423791936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -412,13 +416,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359961168"/>
+        <c:crossAx val="423768416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359961168"/>
+        <c:axId val="423768416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -537,7 +541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359356112"/>
+        <c:crossAx val="423791936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -783,11 +787,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="414403376"/>
-        <c:axId val="412304384"/>
+        <c:axId val="423788576"/>
+        <c:axId val="423787456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="414403376"/>
+        <c:axId val="423788576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -844,12 +848,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="412304384"/>
+        <c:crossAx val="423787456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="412304384"/>
+        <c:axId val="423787456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -907,7 +911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414403376"/>
+        <c:crossAx val="423788576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1172,11 +1176,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="349396704"/>
-        <c:axId val="359315216"/>
+        <c:axId val="423796416"/>
+        <c:axId val="423795296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="349396704"/>
+        <c:axId val="423796416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,12 +1237,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359315216"/>
+        <c:crossAx val="423795296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359315216"/>
+        <c:axId val="423795296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,7 +1299,459 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349396704"/>
+        <c:crossAx val="423796416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LOOCV DATA'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:forward val="100"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'LOOCV DATA'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>280</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'LOOCV DATA'!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.324324</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51351400000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.48648599999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48648599999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56756799999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48648599999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.51351400000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48648599999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54054100000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56756799999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56756799999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="423801456"/>
+        <c:axId val="423767856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="423801456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Number of Days of Data</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423767856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="423767856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>LOOCV Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423801456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1464,6 +1920,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2497,6 +2993,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3091,6 +4103,41 @@
       <xdr:colOff>528637</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>424543</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>503464</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3377,8 +4424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3408,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>I2*$G$4</f>
+        <f t="shared" ref="B2:B12" si="0">I2*$G$4</f>
         <v>7</v>
       </c>
       <c r="C2" s="1">
@@ -3429,7 +4476,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>I3*$G$4</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C3" s="1">
@@ -3451,7 +4498,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f>I4*$G$4</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C4" s="1">
@@ -3473,7 +4520,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>I5*$G$4</f>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="C5" s="1">
@@ -3488,7 +4535,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <f>I6*$G$4</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C6" s="1">
@@ -3503,7 +4550,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <f>I7*$G$4</f>
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="C7" s="1">
@@ -3518,7 +4565,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <f>I8*$G$4</f>
+        <f t="shared" si="0"/>
         <v>112</v>
       </c>
       <c r="C8" s="1">
@@ -3533,7 +4580,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <f>I9*$G$4</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="C9" s="1">
@@ -3548,7 +4595,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <f>I10*$G$4</f>
+        <f t="shared" si="0"/>
         <v>168</v>
       </c>
       <c r="C10" s="1">
@@ -3563,7 +4610,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <f>I11*$G$4</f>
+        <f t="shared" si="0"/>
         <v>224</v>
       </c>
       <c r="C11" s="1">
@@ -3578,7 +4625,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <f>I12*$G$4</f>
+        <f t="shared" si="0"/>
         <v>280</v>
       </c>
       <c r="C12" s="1">
@@ -3619,7 +4666,7 @@
         <v>1</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:B45" si="0">I3*$G$4</f>
+        <f t="shared" ref="B36:B45" si="1">I3*$G$4</f>
         <v>14</v>
       </c>
       <c r="C36" s="1">
@@ -3631,7 +4678,7 @@
         <v>2</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C37" s="1">
@@ -3643,7 +4690,7 @@
         <v>3</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="C38" s="1">
@@ -3655,7 +4702,7 @@
         <v>4</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="C39" s="1">
@@ -3667,7 +4714,7 @@
         <v>5</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="C40" s="1">
@@ -3679,7 +4726,7 @@
         <v>6</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>112</v>
       </c>
       <c r="C41" s="1">
@@ -3691,7 +4738,7 @@
         <v>7</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
       <c r="C42" s="1">
@@ -3703,7 +4750,7 @@
         <v>8</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>168</v>
       </c>
       <c r="C43" s="1">
@@ -3715,7 +4762,7 @@
         <v>9</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>224</v>
       </c>
       <c r="C44" s="1">
@@ -3727,7 +4774,7 @@
         <v>10</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="C45" s="1">
@@ -3745,7 +4792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -3810,7 +4857,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A22" si="0">A3-5</f>
+        <f t="shared" ref="A4:A15" si="0">A3-5</f>
         <v>59</v>
       </c>
       <c r="B4" s="1">
@@ -3823,7 +4870,7 @@
         <v>0.932203</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E21" si="1">AVERAGE(B4:D4)</f>
+        <f t="shared" ref="E4:E15" si="1">AVERAGE(B4:D4)</f>
         <v>0.94351866666666673</v>
       </c>
     </row>
@@ -4105,6 +5152,242 @@
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11:M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B12" si="0">I2*$G$4</f>
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.324324</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>365.24</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.51351400000000003</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <f>G2/12</f>
+        <v>30.436666666666667</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.48648599999999997</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <f>7</f>
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.48648599999999997</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.56756799999999996</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.48648599999999997</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.51351400000000003</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.48648599999999997</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.54054100000000005</v>
+      </c>
+      <c r="I10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>224</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.56756799999999996</v>
+      </c>
+      <c r="I11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.56756799999999996</v>
+      </c>
+      <c r="I12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <f>2*G3</f>
+        <v>60.873333333333335</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.43243200000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>4*G3</f>
+        <v>121.74666666666667</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.43243200000000004</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Data analysis, powerpoint, edits
</commit_message>
<xml_diff>
--- a/DataFiles/Data_study/Data_analysis.xlsx
+++ b/DataFiles/Data_study/Data_analysis.xlsx
@@ -293,11 +293,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="423791936"/>
-        <c:axId val="423768416"/>
+        <c:axId val="267439776"/>
+        <c:axId val="333848336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="423791936"/>
+        <c:axId val="267439776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -416,13 +416,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423768416"/>
+        <c:crossAx val="333848336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="423768416"/>
+        <c:axId val="333848336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -541,7 +541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423791936"/>
+        <c:crossAx val="267439776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -605,7 +605,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -787,11 +786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="423788576"/>
-        <c:axId val="423787456"/>
+        <c:axId val="327752592"/>
+        <c:axId val="327753152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="423788576"/>
+        <c:axId val="327752592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,12 +847,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423787456"/>
+        <c:crossAx val="327753152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="423787456"/>
+        <c:axId val="327753152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -911,7 +910,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423788576"/>
+        <c:crossAx val="327752592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1176,11 +1175,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="423796416"/>
-        <c:axId val="423795296"/>
+        <c:axId val="327755392"/>
+        <c:axId val="333260864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="423796416"/>
+        <c:axId val="327755392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,12 +1236,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423795296"/>
+        <c:crossAx val="333260864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="423795296"/>
+        <c:axId val="333260864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1298,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423796416"/>
+        <c:crossAx val="327755392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1515,11 +1514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="423801456"/>
-        <c:axId val="423767856"/>
+        <c:axId val="333263104"/>
+        <c:axId val="333263664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="423801456"/>
+        <c:axId val="333263104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1558,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:rPr lang="en-US" sz="2200"/>
                   <a:t>Number of Days of Data</a:t>
                 </a:r>
               </a:p>
@@ -1617,7 +1616,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1632,12 +1631,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423767856"/>
+        <c:crossAx val="333263664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="423767856"/>
+        <c:axId val="333263664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -1665,7 +1664,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1678,7 +1677,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:rPr lang="en-US" sz="2200" baseline="0"/>
                   <a:t>LOOCV Accuracy</a:t>
                 </a:r>
               </a:p>
@@ -1698,7 +1697,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1736,7 +1735,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1751,7 +1750,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423801456"/>
+        <c:crossAx val="333263104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4130,12 +4129,12 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>424543</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>503464</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>34476</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -4792,7 +4791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -5163,8 +5162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11:M17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>